<commit_message>
Esquema Base de datos inventarios
</commit_message>
<xml_diff>
--- a/consulta_sesion.xlsx
+++ b/consulta_sesion.xlsx
@@ -508,27 +508,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>050188</t>
+          <t>035148</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9050177</t>
+          <t>9014224</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>23268523700017</t>
+          <t>001AE87EB516</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>LECTOR DE CODIGO DE BARRAS</t>
+          <t>TELEFONO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>LAURA MILENA PEÑARANDA CAMARGO</t>
+          <t>JORGE ANDRES MELO MAYORGA</t>
         </is>
       </c>
     </row>

</xml_diff>